<commit_message>
20.11.2023 hoan thanh book data
</commit_message>
<xml_diff>
--- a/data/category_book.xlsx
+++ b/data/category_book.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A533E-851C-42DA-A098-9640FE55F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0F6ED1-00A9-4B8A-95CB-7F528A4463C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="0" windowWidth="13140" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,86 +459,103 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>